<commit_message>
Fixed goal for exp B map 2
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/SimulinkConfigExpBmap2goal1.xlsx
+++ b/AD-EYE/TA/Configurations/SimulinkConfigExpBmap2goal1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49733E85-4281-4A22-9428-849E8ADC26B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDDFC92-6F90-415F-B890-CB4F6BA7898C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3216" yWindow="2556" windowWidth="14724" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14712" yWindow="3600" windowWidth="14724" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>255</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Experiment B files
</commit_message>
<xml_diff>
--- a/AD-EYE/TA/Configurations/SimulinkConfigExpBmap2goal1.xlsx
+++ b/AD-EYE/TA/Configurations/SimulinkConfigExpBmap2goal1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\TA\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49733E85-4281-4A22-9428-849E8ADC26B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDDFC92-6F90-415F-B890-CB4F6BA7898C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3216" yWindow="2556" windowWidth="14724" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14712" yWindow="3600" windowWidth="14724" windowHeight="12204" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>255</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>